<commit_message>
Implemented BPI Calculator in Java
</commit_message>
<xml_diff>
--- a/python/csvs/WyomingCountyData.xlsx
+++ b/python/csvs/WyomingCountyData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Banzhaf\python\csvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EF266EC-A6E4-4AEF-A6D2-B9536EE42ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207C2CA0-1F02-4B1C-9194-66EC0FD2FB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,47 @@
     <sheet name="500" sheetId="5" r:id="rId5"/>
     <sheet name="Best" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
   <si>
     <t>50% BPI Sum</t>
   </si>
@@ -65,16 +100,30 @@
   <si>
     <t xml:space="preserve"> 2/3 BPI Diff</t>
   </si>
+  <si>
+    <t>2/3 Absolute Value</t>
+  </si>
+  <si>
+    <t>Top 2 2/3</t>
+  </si>
+  <si>
+    <t>50% Absolute Value</t>
+  </si>
+  <si>
+    <t>Top 2 50%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000%"/>
+    <numFmt numFmtId="171" formatCode="0.00000000"/>
+    <numFmt numFmtId="181" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +257,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF454545"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -551,13 +606,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -912,11 +972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,10 +988,14 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,31 +1003,34 @@
         <v>4.9030227000000003E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1.0359607E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f>K9</f>
+        <v>1.0359606550000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>4.2095150999999997E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.0763620999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>M9</f>
+        <v>1.0763621080000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -971,7 +1038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -996,8 +1063,21 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1022,8 +1102,25 @@
       <c r="H7" s="2">
         <v>-1.4901310400000001E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" cm="1">
+        <f t="array" ref="J7:J22">ABS(F7:F22)</f>
+        <v>5.7160910699999995E-4</v>
+      </c>
+      <c r="K7">
+        <f xml:space="preserve"> LARGE(J6:J21,1)</f>
+        <v>5.1804665400000003E-3</v>
+      </c>
+      <c r="L7" s="2" cm="1">
+        <f t="array" ref="L7:L22">ABS(H7:H22)</f>
+        <v>1.4901310400000001E-3</v>
+      </c>
+      <c r="M7">
+        <f xml:space="preserve"> LARGE(L6:L21,1)</f>
+        <v>6.3975508200000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1048,8 +1145,23 @@
       <c r="H8" s="2">
         <v>1.5400931799999999E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <v>1.35085711E-3</v>
+      </c>
+      <c r="K8">
+        <f xml:space="preserve"> LARGE(J7:J22,2)</f>
+        <v>5.1791400099999996E-3</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1.5400931799999999E-3</v>
+      </c>
+      <c r="M8">
+        <f xml:space="preserve"> LARGE(L7:L22,2)</f>
+        <v>4.3660702600000004E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1074,8 +1186,23 @@
       <c r="H9" s="2">
         <v>4.1676540099999998E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
+        <v>3.1780245099999999E-3</v>
+      </c>
+      <c r="K9">
+        <f>SUM(K7:K8)</f>
+        <v>1.0359606550000001E-2</v>
+      </c>
+      <c r="L9" s="2">
+        <v>4.1676540099999998E-3</v>
+      </c>
+      <c r="M9">
+        <f>SUM(M7:M8)</f>
+        <v>1.0763621080000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1100,8 +1227,17 @@
       <c r="H10" s="2">
         <v>-2.1302205699999998E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
+        <v>3.6892727999999998E-3</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="2">
+        <v>2.1302205699999998E-3</v>
+      </c>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1126,8 +1262,15 @@
       <c r="H11" s="2">
         <v>-3.31417454E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
+        <v>4.3554279499999999E-3</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3.31417454E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1152,8 +1295,15 @@
       <c r="H12" s="2">
         <v>4.6503448599999998E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <v>5.7621892499999997E-4</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4.6503448599999998E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1178,8 +1328,15 @@
       <c r="H13" s="2">
         <v>6.3975508200000003E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>4.8073343700000002E-3</v>
+      </c>
+      <c r="L13" s="2">
+        <v>6.3975508200000003E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1204,8 +1361,15 @@
       <c r="H14" s="2">
         <v>-7.9463578200000004E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2">
+        <v>1.09774484E-3</v>
+      </c>
+      <c r="L14" s="2">
+        <v>7.9463578200000004E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1230,8 +1394,15 @@
       <c r="H15" s="2">
         <v>-2.7442489400000001E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
+        <v>3.7284085000000001E-3</v>
+      </c>
+      <c r="L15" s="2">
+        <v>2.7442489400000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1256,8 +1427,15 @@
       <c r="H16" s="2">
         <v>4.3660702600000004E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
+        <v>3.1302423200000001E-3</v>
+      </c>
+      <c r="L16" s="2">
+        <v>4.3660702600000004E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1282,8 +1460,15 @@
       <c r="H17" s="2">
         <v>-4.1392131299999996E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
+        <v>5.1804665400000003E-3</v>
+      </c>
+      <c r="L17" s="2">
+        <v>4.1392131299999996E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1308,8 +1493,15 @@
       <c r="H18" s="2">
         <v>-7.2355290000000001E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
+        <v>3.7995960499999999E-3</v>
+      </c>
+      <c r="L18" s="2">
+        <v>7.2355290000000001E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1334,8 +1526,15 @@
       <c r="H19" s="2">
         <v>4.1111727700000001E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
+        <v>3.0699193599999998E-3</v>
+      </c>
+      <c r="L19" s="2">
+        <v>4.1111727700000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -1360,8 +1559,15 @@
       <c r="H20" s="2">
         <v>-2.8641727100000001E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
+        <v>4.4543891599999998E-3</v>
+      </c>
+      <c r="L20" s="2">
+        <v>2.8641727100000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -1386,8 +1592,15 @@
       <c r="H21" s="2">
         <v>-2.8409985499999999E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <v>5.1791400099999996E-3</v>
+      </c>
+      <c r="L21" s="2">
+        <v>2.8409985499999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -1412,18 +1625,26 @@
       <c r="H22" s="2">
         <v>-6.2273507900000003E-6</v>
       </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2">
+        <v>8.6157589499999995E-4</v>
+      </c>
+      <c r="L22" s="2">
+        <v>6.2273507900000003E-6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A6:H6"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,10 +1656,12 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1669,7 @@
         <v>1.7781508000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1454,23 +1677,25 @@
         <v>4.8462840000000002E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>3.7657164E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.4734545999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>L9</f>
+        <v>1.4734545660000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1478,7 +1703,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1503,8 +1728,16 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1529,8 +1762,24 @@
       <c r="H7" s="2">
         <v>-2.03151179E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" cm="1">
+        <f t="array" ref="I7:I22">ABS(F7:F22)</f>
+        <v>3.2837309600000002E-4</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> LARGE(I6:I21,1)</f>
+        <v>3.1376958399999999E-3</v>
+      </c>
+      <c r="K7" s="2" cm="1">
+        <f t="array" ref="K7:K22">ABS(H7:H22)</f>
+        <v>2.03151179E-3</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> LARGE(K6:K21,1)</f>
+        <v>8.4126555700000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1555,8 +1804,22 @@
       <c r="H8" s="2">
         <v>1.45244091E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>1.5956816299999999E-3</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> LARGE(I7:I22,2)</f>
+        <v>1.7708635999999999E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.45244091E-3</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> LARGE(K7:K22,2)</f>
+        <v>6.3218900899999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1581,8 +1844,22 @@
       <c r="H9" s="2">
         <v>-1.0912415100000001E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>1.70858807E-3</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J7:J8)</f>
+        <v>4.9085594399999998E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.0912415100000001E-3</v>
+      </c>
+      <c r="L9">
+        <f>SUM(L7:L8)</f>
+        <v>1.4734545660000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1607,8 +1884,19 @@
       <c r="H10" s="2">
         <v>2.8509270299999999E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>1.668428E-3</v>
+      </c>
+      <c r="J10" s="5">
+        <f>J9-B2</f>
+        <v>6.2275439999999634E-5</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2.8509270299999999E-3</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1633,8 +1921,14 @@
       <c r="H11" s="2">
         <v>1.9626206899999998E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>5.5080646600000002E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.9626206899999998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1659,8 +1953,14 @@
       <c r="H12" s="2">
         <v>4.7675337299999998E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>5.0844244299999997E-4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>4.7675337299999998E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1685,8 +1985,14 @@
       <c r="H13" s="2">
         <v>1.62397395E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>3.5858394300000001E-5</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.62397395E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1711,8 +2017,14 @@
       <c r="H14" s="2">
         <v>-5.8010456800000002E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1.1489224899999999E-3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>5.8010456800000002E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1737,8 +2049,14 @@
       <c r="H15" s="2">
         <v>2.79499647E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>1.1351641200000001E-3</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2.79499647E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1763,8 +2081,14 @@
       <c r="H16" s="2">
         <v>-3.2619604599999998E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>1.7380102699999999E-3</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3.2619604599999998E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1789,8 +2113,14 @@
       <c r="H17" s="2">
         <v>1.1375821000000001E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>2.74232125E-4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.1375821000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1815,8 +2145,14 @@
       <c r="H18" s="2">
         <v>-6.3218900899999998E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>1.7708635999999999E-3</v>
+      </c>
+      <c r="K18" s="2">
+        <v>6.3218900899999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1841,8 +2177,14 @@
       <c r="H19" s="2">
         <v>4.12289166E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>3.1376958399999999E-3</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4.12289166E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -1867,8 +2209,14 @@
       <c r="H20" s="2">
         <v>2.4063960600000001E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>8.0297772899999998E-4</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2.4063960600000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -1893,8 +2241,14 @@
       <c r="H21" s="2">
         <v>-8.4126555700000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>6.3581044900000005E-4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>8.4126555700000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -1918,6 +2272,12 @@
       </c>
       <c r="H22" s="2">
         <v>-6.4982671600000001E-5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>7.4165285500000003E-4</v>
+      </c>
+      <c r="K22" s="2">
+        <v>6.4982671600000001E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1926,11 +2286,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A6:H6"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,10 +2302,12 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1953,7 +2315,7 @@
         <v>1.2388450000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1961,23 +2323,25 @@
         <v>3.2390299999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>2.9520879999999999E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.0605776000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>L9</f>
+        <v>1.204424269E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +2349,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2010,8 +2374,16 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2036,8 +2408,24 @@
       <c r="H7" s="2">
         <v>-1.9585680199999999E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" cm="1">
+        <f t="array" ref="I7:I22">ABS(F7:F22)</f>
+        <v>4.7804323299999998E-4</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> LARGE(I6:I21,1)</f>
+        <v>1.72285866E-3</v>
+      </c>
+      <c r="K7" s="2" cm="1">
+        <f t="array" ref="K7:K22">ABS(H7:H22)</f>
+        <v>1.9585680199999999E-3</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> LARGE(K6:K21,1)</f>
+        <v>7.3600123099999996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2062,8 +2450,22 @@
       <c r="H8" s="2">
         <v>1.4877350400000001E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>1.51617132E-3</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> LARGE(I7:I22,2)</f>
+        <v>1.51617132E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.4877350400000001E-3</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> LARGE(K7:K22,2)</f>
+        <v>4.6842303800000004E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2088,8 +2490,22 @@
       <c r="H9" s="2">
         <v>2.9483845599999998E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>4.60163862E-4</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J7:J8)</f>
+        <v>3.23902998E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2.9483845599999998E-4</v>
+      </c>
+      <c r="L9">
+        <f>SUM(L7:L8)</f>
+        <v>1.204424269E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2114,8 +2530,19 @@
       <c r="H10" s="2">
         <v>1.3895111E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>2.3413540600000001E-4</v>
+      </c>
+      <c r="J10" s="5">
+        <f>J9-B2</f>
+        <v>-1.9999999920083944E-11</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.3895111E-3</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2140,8 +2567,14 @@
       <c r="H11" s="2">
         <v>5.6605107299999996E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>1.0330494799999999E-3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5.6605107299999996E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -2166,8 +2599,14 @@
       <c r="H12" s="2">
         <v>5.1463154799999996E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>5.4390312300000004E-4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5.1463154799999996E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -2192,8 +2631,14 @@
       <c r="H13" s="2">
         <v>3.2457640700000001E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>1.72285866E-3</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3.2457640700000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -2218,8 +2663,14 @@
       <c r="H14" s="2">
         <v>-7.5762952899999995E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1.0791274599999999E-3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>7.5762952899999995E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -2244,8 +2695,14 @@
       <c r="H15" s="2">
         <v>1.3275700100000001E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>5.0808839000000003E-4</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.3275700100000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -2270,8 +2727,14 @@
       <c r="H16" s="2">
         <v>1.2840718E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>5.4184928300000002E-5</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.2840718E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2296,8 +2759,14 @@
       <c r="H17" s="2">
         <v>2.7478499499999998E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>1.40959322E-3</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2.7478499499999998E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -2322,8 +2791,14 @@
       <c r="H18" s="2">
         <v>-4.6842303800000004E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>1.5940492800000001E-4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4.6842303800000004E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -2348,8 +2823,14 @@
       <c r="H19" s="2">
         <v>1.0715532600000001E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>1.4306474600000001E-4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.0715532600000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2374,8 +2855,14 @@
       <c r="H20" s="2">
         <v>8.2150655400000001E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>9.5873954100000002E-4</v>
+      </c>
+      <c r="K20" s="2">
+        <v>8.2150655400000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2400,8 +2887,14 @@
       <c r="H21" s="2">
         <v>-7.3600123099999996E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>1.3861968300000001E-3</v>
+      </c>
+      <c r="K21" s="2">
+        <v>7.3600123099999996E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2424,6 +2917,12 @@
         <v>2.0182881600000001E-2</v>
       </c>
       <c r="H22" s="2">
+        <v>9.3573757300000002E-6</v>
+      </c>
+      <c r="I22" s="2">
+        <v>7.0172478300000005E-4</v>
+      </c>
+      <c r="K22" s="2">
         <v>9.3573757300000002E-6</v>
       </c>
     </row>
@@ -2433,11 +2932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A6:H6"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,10 +2948,12 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2460,7 +2961,7 @@
         <v>1.1558242999999999E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2468,23 +2969,25 @@
         <v>2.7974950000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>3.4428743999999997E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.1984776000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>L9</f>
+        <v>1.304366144E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +2995,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2517,8 +3020,16 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2543,8 +3054,24 @@
       <c r="H7" s="2">
         <v>-2.0296321499999998E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" cm="1">
+        <f t="array" ref="I7:I22">ABS(F7:F22)</f>
+        <v>4.69526151E-4</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> LARGE(I6:I21,1)</f>
+        <v>1.43483146E-3</v>
+      </c>
+      <c r="K7" s="2" cm="1">
+        <f t="array" ref="K7:K22">ABS(H7:H22)</f>
+        <v>2.0296321499999998E-3</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> LARGE(K6:K21,1)</f>
+        <v>9.0006356899999997E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2569,8 +3096,22 @@
       <c r="H8" s="2">
         <v>-1.4772117799999999E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>1.43483146E-3</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> LARGE(I7:I22,2)</f>
+        <v>1.3626631499999999E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.4772117799999999E-3</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> LARGE(K7:K22,2)</f>
+        <v>4.04302575E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2595,8 +3136,22 @@
       <c r="H9" s="2">
         <v>9.2277950800000001E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>2.89956234E-4</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J7:J8)</f>
+        <v>2.7974946099999999E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>9.2277950800000001E-4</v>
+      </c>
+      <c r="L9">
+        <f>SUM(L7:L8)</f>
+        <v>1.304366144E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2621,8 +3176,19 @@
       <c r="H10" s="2">
         <v>5.4147771000000004E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>1.0297020800000001E-3</v>
+      </c>
+      <c r="J10" s="5">
+        <f>J9-B2</f>
+        <v>-3.9000000017636038E-10</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5.4147771000000004E-4</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2647,8 +3213,14 @@
       <c r="H11" s="2">
         <v>1.6681049300000001E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>4.2638054600000001E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.6681049300000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -2673,8 +3245,14 @@
       <c r="H12" s="2">
         <v>1.20224273E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>1.2409105699999999E-4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.20224273E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -2699,8 +3277,14 @@
       <c r="H13" s="2">
         <v>1.8131177599999999E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>8.1454487000000002E-5</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.8131177599999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -2725,8 +3309,14 @@
       <c r="H14" s="2">
         <v>-6.6386650799999997E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1.0953099700000001E-3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>6.6386650799999997E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -2751,8 +3341,14 @@
       <c r="H15" s="2">
         <v>2.9841402799999999E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>1.2524770000000001E-3</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2.9841402799999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -2777,8 +3373,14 @@
       <c r="H16" s="2">
         <v>2.2773656699999999E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>7.9339883699999997E-4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2.2773656699999999E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2803,8 +3405,14 @@
       <c r="H17" s="2">
         <v>8.4306633800000001E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>3.9865804400000002E-4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>8.4306633800000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -2829,8 +3437,14 @@
       <c r="H18" s="2">
         <v>-4.04302575E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>1.3626631499999999E-3</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4.04302575E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -2855,8 +3469,14 @@
       <c r="H19" s="2">
         <v>1.90948555E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>6.8766867400000002E-4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.90948555E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2881,8 +3501,14 @@
       <c r="H20" s="2">
         <v>2.5518024099999998E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>8.8512252299999998E-4</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2.5518024099999998E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2907,8 +3533,14 @@
       <c r="H21" s="2">
         <v>-9.0006356899999997E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>7.7137966400000005E-4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>9.0006356899999997E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2931,6 +3563,12 @@
         <v>2.0674313199999999E-2</v>
       </c>
       <c r="H22" s="2">
+        <v>5.00788992E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <v>4.5562302500000001E-4</v>
+      </c>
+      <c r="K22" s="2">
         <v>5.00788992E-4</v>
       </c>
     </row>
@@ -2940,11 +3578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A6:H6"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,10 +3594,12 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2967,7 +3607,7 @@
         <v>1.0206845000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2975,23 +3615,25 @@
         <v>2.1976349999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>3.1587522E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.0678606E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>L9</f>
+        <v>1.3330325649999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2999,7 +3641,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3024,8 +3666,16 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3050,8 +3700,24 @@
       <c r="H7" s="2">
         <v>-1.90381773E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" cm="1">
+        <f t="array" ref="I7:I22">ABS(F7:F22)</f>
+        <v>4.2122404800000002E-4</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> LARGE(I6:I21,1)</f>
+        <v>1.3455509599999999E-3</v>
+      </c>
+      <c r="K7" s="2" cm="1">
+        <f t="array" ref="K7:K22">ABS(H7:H22)</f>
+        <v>1.90381773E-3</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> LARGE(K6:K21,1)</f>
+        <v>7.9613271999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3076,8 +3742,22 @@
       <c r="H8" s="2">
         <v>-5.5961741799999995E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>5.54628444E-4</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> LARGE(I7:I22,2)</f>
+        <v>8.52083761E-4</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5.5961741799999995E-4</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> LARGE(K7:K22,2)</f>
+        <v>5.3689984499999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3102,8 +3782,22 @@
       <c r="H9" s="2">
         <v>9.9555003800000006E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>8.3247521099999997E-4</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J7:J8)</f>
+        <v>2.1976347209999997E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>9.9555003800000006E-5</v>
+      </c>
+      <c r="L9">
+        <f>SUM(L7:L8)</f>
+        <v>1.3330325649999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3128,8 +3822,19 @@
       <c r="H10" s="2">
         <v>2.1401162799999998E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>4.20378626E-4</v>
+      </c>
+      <c r="J10" s="5">
+        <f>J9-B2</f>
+        <v>-2.7900000018621363E-10</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2.1401162799999998E-3</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3154,8 +3859,14 @@
       <c r="H11" s="2">
         <v>1.0233866299999999E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>4.2598429199999999E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.0233866299999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -3180,8 +3891,14 @@
       <c r="H12" s="2">
         <v>2.4133062599999999E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>1.3455509599999999E-3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2.4133062599999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -3206,8 +3923,14 @@
       <c r="H13" s="2">
         <v>2.7172787500000001E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>8.4814756499999996E-4</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.7172787500000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -3232,8 +3955,14 @@
       <c r="H14" s="2">
         <v>1.26213993E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>8.52083761E-4</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.26213993E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -3258,8 +3987,14 @@
       <c r="H15" s="2">
         <v>1.78737439E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>1.6764870999999999E-4</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.78737439E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -3284,8 +4019,14 @@
       <c r="H16" s="2">
         <v>5.0593961499999999E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>6.6251227900000005E-4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>5.0593961499999999E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -3310,8 +4051,14 @@
       <c r="H17" s="2">
         <v>1.9697177600000002E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>8.0126586500000002E-4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.9697177600000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -3336,8 +4083,14 @@
       <c r="H18" s="2">
         <v>-5.3689984499999998E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>4.0560156399999998E-4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>5.3689984499999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -3362,8 +4115,14 @@
       <c r="H19" s="2">
         <v>4.5697287099999998E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>6.74412296E-4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4.5697287099999998E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -3388,8 +4147,14 @@
       <c r="H20" s="2">
         <v>1.28253771E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>2.9365092100000002E-4</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.28253771E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -3414,8 +4179,14 @@
       <c r="H21" s="2">
         <v>-7.9613271999999999E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>6.6834711100000001E-4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>7.9613271999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -3438,6 +4209,12 @@
         <v>2.0308959800000002E-2</v>
       </c>
       <c r="H22" s="2">
+        <v>1.3543558999999999E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <v>8.32933543E-4</v>
+      </c>
+      <c r="K22" s="2">
         <v>1.3543558999999999E-4</v>
       </c>
     </row>
@@ -3447,11 +4224,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A6:H6"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,10 +4240,12 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3474,7 +4253,7 @@
         <v>1.0206845000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3482,23 +4261,25 @@
         <v>2.1976349999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>3.1587522E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.0678606E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>L9</f>
+        <v>1.3330325649999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3506,7 +4287,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3531,8 +4312,16 @@
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3557,8 +4346,24 @@
       <c r="H7" s="2">
         <v>-1.90381773E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" cm="1">
+        <f t="array" ref="I7:I22">ABS(F7:F22)</f>
+        <v>4.2122404800000002E-4</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> LARGE(I6:I21,1)</f>
+        <v>1.3455509599999999E-3</v>
+      </c>
+      <c r="K7" s="2" cm="1">
+        <f t="array" ref="K7:K22">ABS(H7:H22)</f>
+        <v>1.90381773E-3</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> LARGE(K6:K21,1)</f>
+        <v>7.9613271999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3583,8 +4388,22 @@
       <c r="H8" s="2">
         <v>-5.5961741799999995E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>5.54628444E-4</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> LARGE(I7:I22,2)</f>
+        <v>8.52083761E-4</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5.5961741799999995E-4</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> LARGE(K7:K22,2)</f>
+        <v>5.3689984499999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3609,8 +4428,22 @@
       <c r="H9" s="2">
         <v>9.9555003800000006E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>8.3247521099999997E-4</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J7:J8)</f>
+        <v>2.1976347209999997E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>9.9555003800000006E-5</v>
+      </c>
+      <c r="L9">
+        <f>SUM(L7:L8)</f>
+        <v>1.3330325649999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3635,8 +4468,19 @@
       <c r="H10" s="2">
         <v>2.1401162799999998E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>4.20378626E-4</v>
+      </c>
+      <c r="J10" s="5">
+        <f>J9-B2</f>
+        <v>-2.7900000018621363E-10</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2.1401162799999998E-3</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3661,8 +4505,14 @@
       <c r="H11" s="2">
         <v>1.0233866299999999E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>4.2598429199999999E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.0233866299999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -3687,8 +4537,14 @@
       <c r="H12" s="2">
         <v>2.4133062599999999E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>1.3455509599999999E-3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2.4133062599999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -3713,8 +4569,14 @@
       <c r="H13" s="2">
         <v>2.7172787500000001E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>8.4814756499999996E-4</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.7172787500000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -3739,8 +4601,14 @@
       <c r="H14" s="2">
         <v>1.26213993E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>8.52083761E-4</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.26213993E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -3765,8 +4633,14 @@
       <c r="H15" s="2">
         <v>1.78737439E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>1.6764870999999999E-4</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.78737439E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -3791,8 +4665,14 @@
       <c r="H16" s="2">
         <v>5.0593961499999999E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>6.6251227900000005E-4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>5.0593961499999999E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -3817,8 +4697,14 @@
       <c r="H17" s="2">
         <v>1.9697177600000002E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>8.0126586500000002E-4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.9697177600000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -3843,8 +4729,14 @@
       <c r="H18" s="2">
         <v>-5.3689984499999998E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>4.0560156399999998E-4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>5.3689984499999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -3869,8 +4761,14 @@
       <c r="H19" s="2">
         <v>4.5697287099999998E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>6.74412296E-4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4.5697287099999998E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -3895,8 +4793,14 @@
       <c r="H20" s="2">
         <v>1.28253771E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>2.9365092100000002E-4</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.28253771E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -3921,8 +4825,14 @@
       <c r="H21" s="2">
         <v>-7.9613271999999999E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>6.6834711100000001E-4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>7.9613271999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -3945,6 +4855,12 @@
         <v>2.0308959800000002E-2</v>
       </c>
       <c r="H22" s="2">
+        <v>1.3543558999999999E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <v>8.32933543E-4</v>
+      </c>
+      <c r="K22" s="2">
         <v>1.3543558999999999E-4</v>
       </c>
     </row>

</xml_diff>